<commit_message>
Update the Fee Amendment Form
</commit_message>
<xml_diff>
--- a/GECO/AnnualFees/FeeAmendmentForm.xlsx
+++ b/GECO/AnnualFees/FeeAmendmentForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwaldron\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FFB8471-B480-4C37-A585-CC5B14FA31E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEDB1E2-88DB-43B7-9FA0-7EC1BD1F0826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="930" windowWidth="15585" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -279,10 +279,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-409]&quot;Version: &quot;d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -403,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -608,12 +609,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
@@ -747,7 +759,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -769,7 +780,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -797,19 +807,38 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -823,29 +852,38 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -856,11 +894,11 @@
     <xf numFmtId="44" fontId="2" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -876,113 +914,92 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1564,10 +1581,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AD82"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:L6"/>
     </sheetView>
   </sheetViews>
@@ -1598,37 +1617,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
-      <c r="AC1" s="102"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="152"/>
+      <c r="K1" s="152"/>
+      <c r="L1" s="152"/>
+      <c r="M1" s="152"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="152"/>
+      <c r="P1" s="152"/>
+      <c r="Q1" s="152"/>
+      <c r="R1" s="152"/>
+      <c r="S1" s="152"/>
+      <c r="T1" s="152"/>
+      <c r="U1" s="152"/>
+      <c r="V1" s="152"/>
+      <c r="W1" s="152"/>
+      <c r="X1" s="152"/>
+      <c r="Y1" s="152"/>
+      <c r="Z1" s="152"/>
+      <c r="AA1" s="152"/>
+      <c r="AB1" s="152"/>
+      <c r="AC1" s="152"/>
     </row>
     <row r="2" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="18" t="s">
@@ -1643,23 +1662,23 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="N2" s="118" t="s">
+      <c r="N2" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
-      <c r="AA2" s="118"/>
-      <c r="AB2" s="118"/>
+      <c r="O2" s="155"/>
+      <c r="P2" s="155"/>
+      <c r="Q2" s="155"/>
+      <c r="R2" s="155"/>
+      <c r="S2" s="155"/>
+      <c r="T2" s="155"/>
+      <c r="U2" s="155"/>
+      <c r="V2" s="155"/>
+      <c r="W2" s="155"/>
+      <c r="X2" s="155"/>
+      <c r="Y2" s="155"/>
+      <c r="Z2" s="155"/>
+      <c r="AA2" s="155"/>
+      <c r="AB2" s="155"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="E3" s="18" t="s">
@@ -1674,21 +1693,21 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="118"/>
-      <c r="U3" s="118"/>
-      <c r="V3" s="118"/>
-      <c r="W3" s="118"/>
-      <c r="X3" s="118"/>
-      <c r="Y3" s="118"/>
-      <c r="Z3" s="118"/>
-      <c r="AA3" s="118"/>
-      <c r="AB3" s="118"/>
+      <c r="N3" s="155"/>
+      <c r="O3" s="155"/>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="155"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="155"/>
+      <c r="T3" s="155"/>
+      <c r="U3" s="155"/>
+      <c r="V3" s="155"/>
+      <c r="W3" s="155"/>
+      <c r="X3" s="155"/>
+      <c r="Y3" s="155"/>
+      <c r="Z3" s="155"/>
+      <c r="AA3" s="155"/>
+      <c r="AB3" s="155"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="C4" s="4"/>
@@ -1701,21 +1720,21 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="119"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="119"/>
-      <c r="Y4" s="119"/>
-      <c r="Z4" s="119"/>
-      <c r="AA4" s="119"/>
-      <c r="AB4" s="119"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="156"/>
+      <c r="R4" s="156"/>
+      <c r="S4" s="156"/>
+      <c r="T4" s="156"/>
+      <c r="U4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="156"/>
+      <c r="Z4" s="156"/>
+      <c r="AA4" s="156"/>
+      <c r="AB4" s="156"/>
     </row>
     <row r="5" spans="1:29" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
@@ -1748,152 +1767,152 @@
       <c r="AC5" s="10"/>
     </row>
     <row r="6" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149" t="s">
+      <c r="A6" s="111" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="30"/>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="69" t="s">
+      <c r="D6" s="69"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="153"/>
+      <c r="H6" s="153"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="154"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="103"/>
-      <c r="T6" s="103"/>
-      <c r="U6" s="103"/>
-      <c r="V6" s="103"/>
-      <c r="W6" s="103"/>
-      <c r="X6" s="103"/>
-      <c r="Y6" s="103"/>
-      <c r="Z6" s="103"/>
-      <c r="AA6" s="103"/>
-      <c r="AB6" s="104"/>
+      <c r="O6" s="153"/>
+      <c r="P6" s="153"/>
+      <c r="Q6" s="153"/>
+      <c r="R6" s="153"/>
+      <c r="S6" s="153"/>
+      <c r="T6" s="153"/>
+      <c r="U6" s="153"/>
+      <c r="V6" s="153"/>
+      <c r="W6" s="153"/>
+      <c r="X6" s="153"/>
+      <c r="Y6" s="153"/>
+      <c r="Z6" s="153"/>
+      <c r="AA6" s="153"/>
+      <c r="AB6" s="154"/>
       <c r="AC6" s="31"/>
     </row>
     <row r="7" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="149"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="30"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
-      <c r="Y7" s="67"/>
-      <c r="Z7" s="67"/>
-      <c r="AA7" s="67"/>
-      <c r="AB7" s="67"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="66"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="66"/>
+      <c r="Y7" s="66"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="66"/>
+      <c r="AB7" s="66"/>
       <c r="AC7" s="31"/>
     </row>
     <row r="8" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="149"/>
+      <c r="A8" s="111"/>
       <c r="B8" s="30"/>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="71" t="s">
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
-      <c r="AA8" s="74"/>
-      <c r="AB8" s="75"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="73"/>
+      <c r="AB8" s="74"/>
       <c r="AC8" s="31"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A9" s="149"/>
+      <c r="A9" s="111"/>
       <c r="B9" s="30"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="106"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="107"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
-      <c r="AB9" s="107"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="109"/>
+      <c r="Z9" s="109"/>
+      <c r="AA9" s="109"/>
+      <c r="AB9" s="110"/>
       <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="149"/>
+      <c r="A10" s="111"/>
       <c r="B10" s="30"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
       <c r="M10" s="32"/>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
@@ -1913,265 +1932,265 @@
       <c r="AC10" s="31"/>
     </row>
     <row r="11" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="149"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="30"/>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="72"/>
-      <c r="P11" s="72"/>
-      <c r="Q11" s="72"/>
-      <c r="R11" s="72"/>
-      <c r="S11" s="72"/>
-      <c r="T11" s="72"/>
-      <c r="U11" s="72"/>
-      <c r="V11" s="72"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="74"/>
-      <c r="Y11" s="74"/>
-      <c r="Z11" s="74"/>
-      <c r="AA11" s="74"/>
-      <c r="AB11" s="75"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="71"/>
+      <c r="V11" s="71"/>
+      <c r="W11" s="71"/>
+      <c r="X11" s="73"/>
+      <c r="Y11" s="73"/>
+      <c r="Z11" s="73"/>
+      <c r="AA11" s="73"/>
+      <c r="AB11" s="74"/>
       <c r="AC11" s="31"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A12" s="149"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
-      <c r="AB12" s="107"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
+      <c r="Y12" s="109"/>
+      <c r="Z12" s="109"/>
+      <c r="AA12" s="109"/>
+      <c r="AB12" s="110"/>
       <c r="AC12" s="31"/>
     </row>
     <row r="13" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="149"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="30"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="64"/>
-      <c r="X13" s="64"/>
-      <c r="Y13" s="64"/>
-      <c r="Z13" s="64"/>
-      <c r="AA13" s="64"/>
-      <c r="AB13" s="64"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="63"/>
+      <c r="W13" s="63"/>
+      <c r="X13" s="63"/>
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="63"/>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="63"/>
       <c r="AC13" s="31"/>
     </row>
     <row r="14" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="149"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="72"/>
-      <c r="Q14" s="72"/>
-      <c r="R14" s="72"/>
-      <c r="S14" s="72"/>
-      <c r="T14" s="72"/>
-      <c r="U14" s="72"/>
-      <c r="V14" s="72"/>
-      <c r="W14" s="72"/>
-      <c r="X14" s="74"/>
-      <c r="Y14" s="74"/>
-      <c r="Z14" s="74"/>
-      <c r="AA14" s="74"/>
-      <c r="AB14" s="75"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="71"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="71"/>
+      <c r="V14" s="71"/>
+      <c r="W14" s="71"/>
+      <c r="X14" s="73"/>
+      <c r="Y14" s="73"/>
+      <c r="Z14" s="73"/>
+      <c r="AA14" s="73"/>
+      <c r="AB14" s="74"/>
       <c r="AC14" s="31"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="149"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
-      <c r="O15" s="106"/>
-      <c r="P15" s="106"/>
-      <c r="Q15" s="106"/>
-      <c r="R15" s="106"/>
-      <c r="S15" s="106"/>
-      <c r="T15" s="106"/>
-      <c r="U15" s="106"/>
-      <c r="V15" s="106"/>
-      <c r="W15" s="106"/>
-      <c r="X15" s="106"/>
-      <c r="Y15" s="106"/>
-      <c r="Z15" s="106"/>
-      <c r="AA15" s="106"/>
-      <c r="AB15" s="107"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="109"/>
+      <c r="N15" s="109"/>
+      <c r="O15" s="109"/>
+      <c r="P15" s="109"/>
+      <c r="Q15" s="109"/>
+      <c r="R15" s="109"/>
+      <c r="S15" s="109"/>
+      <c r="T15" s="109"/>
+      <c r="U15" s="109"/>
+      <c r="V15" s="109"/>
+      <c r="W15" s="109"/>
+      <c r="X15" s="109"/>
+      <c r="Y15" s="109"/>
+      <c r="Z15" s="109"/>
+      <c r="AA15" s="109"/>
+      <c r="AB15" s="110"/>
       <c r="AC15" s="31"/>
     </row>
     <row r="16" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="149"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
-      <c r="X16" s="64"/>
-      <c r="Y16" s="64"/>
-      <c r="Z16" s="64"/>
-      <c r="AA16" s="64"/>
-      <c r="AB16" s="64"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="63"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
+      <c r="Y16" s="63"/>
+      <c r="Z16" s="63"/>
+      <c r="AA16" s="63"/>
+      <c r="AB16" s="63"/>
       <c r="AC16" s="31"/>
     </row>
     <row r="17" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="149"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="30"/>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="73"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="72"/>
       <c r="M17" s="32"/>
-      <c r="N17" s="71" t="s">
+      <c r="N17" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="72"/>
-      <c r="U17" s="72"/>
-      <c r="V17" s="73"/>
-      <c r="W17" s="68"/>
-      <c r="X17" s="71" t="s">
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="73"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="67"/>
+      <c r="X17" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="Y17" s="74"/>
-      <c r="Z17" s="74"/>
-      <c r="AA17" s="74"/>
-      <c r="AB17" s="75"/>
+      <c r="Y17" s="73"/>
+      <c r="Z17" s="73"/>
+      <c r="AA17" s="73"/>
+      <c r="AB17" s="74"/>
       <c r="AC17" s="31"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A18" s="149"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="106"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="106"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="107"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="110"/>
       <c r="M18" s="32"/>
-      <c r="N18" s="105"/>
-      <c r="O18" s="106"/>
-      <c r="P18" s="106"/>
-      <c r="Q18" s="106"/>
-      <c r="R18" s="106"/>
-      <c r="S18" s="106"/>
-      <c r="T18" s="106"/>
-      <c r="U18" s="106"/>
-      <c r="V18" s="107"/>
-      <c r="W18" s="86"/>
-      <c r="X18" s="136"/>
-      <c r="Y18" s="137"/>
-      <c r="Z18" s="137"/>
-      <c r="AA18" s="137"/>
-      <c r="AB18" s="138"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="109"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="109"/>
+      <c r="R18" s="109"/>
+      <c r="S18" s="109"/>
+      <c r="T18" s="109"/>
+      <c r="U18" s="109"/>
+      <c r="V18" s="110"/>
+      <c r="W18" s="84"/>
+      <c r="X18" s="130"/>
+      <c r="Y18" s="131"/>
+      <c r="Z18" s="131"/>
+      <c r="AA18" s="131"/>
+      <c r="AB18" s="132"/>
       <c r="AC18" s="31"/>
     </row>
     <row r="19" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="149"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="30"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -2202,75 +2221,75 @@
       <c r="AC19" s="31"/>
     </row>
     <row r="20" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="149"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="30"/>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="72"/>
-      <c r="T20" s="72"/>
-      <c r="U20" s="72"/>
-      <c r="V20" s="72"/>
-      <c r="W20" s="72"/>
-      <c r="X20" s="74"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="74"/>
-      <c r="AB20" s="75"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="71"/>
+      <c r="T20" s="71"/>
+      <c r="U20" s="71"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="71"/>
+      <c r="X20" s="73"/>
+      <c r="Y20" s="73"/>
+      <c r="Z20" s="73"/>
+      <c r="AA20" s="73"/>
+      <c r="AB20" s="74"/>
       <c r="AC20" s="31"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="149"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="106"/>
-      <c r="O21" s="106"/>
-      <c r="P21" s="106"/>
-      <c r="Q21" s="106"/>
-      <c r="R21" s="106"/>
-      <c r="S21" s="106"/>
-      <c r="T21" s="106"/>
-      <c r="U21" s="106"/>
-      <c r="V21" s="106"/>
-      <c r="W21" s="106"/>
-      <c r="X21" s="106"/>
-      <c r="Y21" s="106"/>
-      <c r="Z21" s="106"/>
-      <c r="AA21" s="106"/>
-      <c r="AB21" s="107"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="109"/>
+      <c r="N21" s="109"/>
+      <c r="O21" s="109"/>
+      <c r="P21" s="109"/>
+      <c r="Q21" s="109"/>
+      <c r="R21" s="109"/>
+      <c r="S21" s="109"/>
+      <c r="T21" s="109"/>
+      <c r="U21" s="109"/>
+      <c r="V21" s="109"/>
+      <c r="W21" s="109"/>
+      <c r="X21" s="109"/>
+      <c r="Y21" s="109"/>
+      <c r="Z21" s="109"/>
+      <c r="AA21" s="109"/>
+      <c r="AB21" s="110"/>
       <c r="AC21" s="31"/>
     </row>
     <row r="22" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="149"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="30"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
-      <c r="E22" s="64"/>
+      <c r="E22" s="63"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
@@ -2297,71 +2316,71 @@
       <c r="AC22" s="31"/>
     </row>
     <row r="23" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="149"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="72"/>
-      <c r="T23" s="72"/>
-      <c r="U23" s="72"/>
-      <c r="V23" s="72"/>
-      <c r="W23" s="72"/>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
-      <c r="Z23" s="74"/>
-      <c r="AA23" s="74"/>
-      <c r="AB23" s="75"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71"/>
+      <c r="V23" s="71"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="73"/>
+      <c r="Y23" s="73"/>
+      <c r="Z23" s="73"/>
+      <c r="AA23" s="73"/>
+      <c r="AB23" s="74"/>
       <c r="AC23" s="31"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A24" s="149"/>
+      <c r="A24" s="111"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="106"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="106"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="106"/>
-      <c r="O24" s="106"/>
-      <c r="P24" s="106"/>
-      <c r="Q24" s="106"/>
-      <c r="R24" s="106"/>
-      <c r="S24" s="106"/>
-      <c r="T24" s="106"/>
-      <c r="U24" s="106"/>
-      <c r="V24" s="106"/>
-      <c r="W24" s="106"/>
-      <c r="X24" s="106"/>
-      <c r="Y24" s="106"/>
-      <c r="Z24" s="106"/>
-      <c r="AA24" s="106"/>
-      <c r="AB24" s="107"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="109"/>
+      <c r="M24" s="109"/>
+      <c r="N24" s="109"/>
+      <c r="O24" s="109"/>
+      <c r="P24" s="109"/>
+      <c r="Q24" s="109"/>
+      <c r="R24" s="109"/>
+      <c r="S24" s="109"/>
+      <c r="T24" s="109"/>
+      <c r="U24" s="109"/>
+      <c r="V24" s="109"/>
+      <c r="W24" s="109"/>
+      <c r="X24" s="109"/>
+      <c r="Y24" s="109"/>
+      <c r="Z24" s="109"/>
+      <c r="AA24" s="109"/>
+      <c r="AB24" s="110"/>
       <c r="AC24" s="31"/>
     </row>
     <row r="25" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="149"/>
+      <c r="A25" s="111"/>
       <c r="B25" s="30"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -2392,73 +2411,73 @@
       <c r="AC25" s="31"/>
     </row>
     <row r="26" spans="1:29" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="149"/>
+      <c r="A26" s="111"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="75"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="74"/>
       <c r="O26" s="32"/>
-      <c r="P26" s="71" t="s">
+      <c r="P26" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="74"/>
-      <c r="T26" s="74"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="72"/>
-      <c r="W26" s="72"/>
-      <c r="X26" s="74"/>
-      <c r="Y26" s="74"/>
-      <c r="Z26" s="74"/>
-      <c r="AA26" s="74"/>
-      <c r="AB26" s="75"/>
+      <c r="Q26" s="71"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="73"/>
+      <c r="V26" s="71"/>
+      <c r="W26" s="71"/>
+      <c r="X26" s="73"/>
+      <c r="Y26" s="73"/>
+      <c r="Z26" s="73"/>
+      <c r="AA26" s="73"/>
+      <c r="AB26" s="74"/>
       <c r="AC26" s="31"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A27" s="149"/>
+      <c r="A27" s="111"/>
       <c r="B27" s="30"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="107"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="110"/>
       <c r="O27" s="33"/>
-      <c r="P27" s="105"/>
-      <c r="Q27" s="106"/>
-      <c r="R27" s="106"/>
-      <c r="S27" s="106"/>
-      <c r="T27" s="106"/>
-      <c r="U27" s="106"/>
-      <c r="V27" s="106"/>
-      <c r="W27" s="106"/>
-      <c r="X27" s="106"/>
-      <c r="Y27" s="106"/>
-      <c r="Z27" s="106"/>
-      <c r="AA27" s="106"/>
-      <c r="AB27" s="107"/>
+      <c r="P27" s="108"/>
+      <c r="Q27" s="109"/>
+      <c r="R27" s="109"/>
+      <c r="S27" s="109"/>
+      <c r="T27" s="109"/>
+      <c r="U27" s="109"/>
+      <c r="V27" s="109"/>
+      <c r="W27" s="109"/>
+      <c r="X27" s="109"/>
+      <c r="Y27" s="109"/>
+      <c r="Z27" s="109"/>
+      <c r="AA27" s="109"/>
+      <c r="AB27" s="110"/>
       <c r="AC27" s="31"/>
     </row>
     <row r="28" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="149"/>
+      <c r="A28" s="111"/>
       <c r="B28" s="30"/>
       <c r="C28" s="12"/>
       <c r="D28" s="38" t="s">
@@ -2553,10 +2572,10 @@
       <c r="AC30" s="12"/>
     </row>
     <row r="31" spans="1:29" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="150" t="s">
+      <c r="A31" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="9"/>
       <c r="D31" s="41"/>
       <c r="E31" s="9"/>
@@ -2586,40 +2605,40 @@
       <c r="AC31" s="10"/>
     </row>
     <row r="32" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="150"/>
+      <c r="A32" s="120"/>
       <c r="B32" s="55"/>
-      <c r="C32" s="139" t="s">
+      <c r="C32" s="133" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="139"/>
-      <c r="E32" s="139"/>
-      <c r="F32" s="139"/>
-      <c r="G32" s="139"/>
-      <c r="H32" s="139"/>
-      <c r="I32" s="140"/>
-      <c r="J32" s="76" t="s">
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="133"/>
+      <c r="H32" s="133"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="K32" s="74"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="123" t="s">
+      <c r="K32" s="73"/>
+      <c r="L32" s="74"/>
+      <c r="M32" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="N32" s="123"/>
-      <c r="O32" s="123"/>
-      <c r="P32" s="123"/>
-      <c r="Q32" s="141"/>
-      <c r="R32" s="76" t="s">
+      <c r="N32" s="129"/>
+      <c r="O32" s="129"/>
+      <c r="P32" s="129"/>
+      <c r="Q32" s="135"/>
+      <c r="R32" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="S32" s="75"/>
-      <c r="T32" s="122" t="s">
+      <c r="S32" s="74"/>
+      <c r="T32" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="U32" s="123"/>
-      <c r="V32" s="123"/>
-      <c r="W32" s="123"/>
-      <c r="X32" s="123"/>
+      <c r="U32" s="129"/>
+      <c r="V32" s="129"/>
+      <c r="W32" s="129"/>
+      <c r="X32" s="129"/>
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
       <c r="AA32" s="12"/>
@@ -2627,30 +2646,30 @@
       <c r="AC32" s="31"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A33" s="150"/>
+      <c r="A33" s="120"/>
       <c r="B33" s="55"/>
-      <c r="C33" s="139"/>
-      <c r="D33" s="139"/>
-      <c r="E33" s="139"/>
-      <c r="F33" s="139"/>
-      <c r="G33" s="139"/>
-      <c r="H33" s="139"/>
-      <c r="I33" s="140"/>
-      <c r="J33" s="144"/>
-      <c r="K33" s="145"/>
-      <c r="L33" s="146"/>
-      <c r="M33" s="123"/>
-      <c r="N33" s="123"/>
-      <c r="O33" s="123"/>
-      <c r="P33" s="123"/>
-      <c r="Q33" s="141"/>
-      <c r="R33" s="120"/>
-      <c r="S33" s="121"/>
-      <c r="T33" s="122"/>
-      <c r="U33" s="123"/>
-      <c r="V33" s="123"/>
-      <c r="W33" s="123"/>
-      <c r="X33" s="123"/>
+      <c r="C33" s="133"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="134"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="138"/>
+      <c r="L33" s="139"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
+      <c r="O33" s="129"/>
+      <c r="P33" s="129"/>
+      <c r="Q33" s="135"/>
+      <c r="R33" s="126"/>
+      <c r="S33" s="127"/>
+      <c r="T33" s="128"/>
+      <c r="U33" s="129"/>
+      <c r="V33" s="129"/>
+      <c r="W33" s="129"/>
+      <c r="X33" s="129"/>
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="12"/>
@@ -2658,7 +2677,7 @@
       <c r="AC33" s="31"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A34" s="150"/>
+      <c r="A34" s="120"/>
       <c r="B34" s="55"/>
       <c r="C34" s="38" t="s">
         <v>68</v>
@@ -2691,7 +2710,7 @@
       <c r="AC34" s="31"/>
     </row>
     <row r="35" spans="1:30" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="150"/>
+      <c r="A35" s="120"/>
       <c r="B35" s="55"/>
       <c r="C35" s="43"/>
       <c r="D35" s="43"/>
@@ -2722,7 +2741,7 @@
       <c r="AC35" s="31"/>
     </row>
     <row r="36" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="150"/>
+      <c r="A36" s="120"/>
       <c r="B36" s="55"/>
       <c r="C36" s="43"/>
       <c r="D36" s="44" t="s">
@@ -2755,7 +2774,7 @@
       <c r="AC36" s="31"/>
     </row>
     <row r="37" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="150"/>
+      <c r="A37" s="120"/>
       <c r="B37" s="55"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -2763,133 +2782,133 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="151" t="s">
+      <c r="I37" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="151"/>
-      <c r="K37" s="151"/>
-      <c r="L37" s="151"/>
-      <c r="M37" s="151"/>
-      <c r="N37" s="151"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="125"/>
+      <c r="L37" s="125"/>
+      <c r="M37" s="125"/>
+      <c r="N37" s="125"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
-      <c r="R37" s="143" t="s">
+      <c r="R37" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="S37" s="143"/>
-      <c r="T37" s="143"/>
-      <c r="U37" s="143"/>
-      <c r="V37" s="143"/>
-      <c r="W37" s="143"/>
-      <c r="X37" s="143"/>
-      <c r="Y37" s="143"/>
-      <c r="Z37" s="143"/>
-      <c r="AA37" s="143"/>
-      <c r="AB37" s="143"/>
+      <c r="S37" s="136"/>
+      <c r="T37" s="136"/>
+      <c r="U37" s="136"/>
+      <c r="V37" s="136"/>
+      <c r="W37" s="136"/>
+      <c r="X37" s="136"/>
+      <c r="Y37" s="136"/>
+      <c r="Z37" s="136"/>
+      <c r="AA37" s="136"/>
+      <c r="AB37" s="136"/>
       <c r="AC37" s="47"/>
       <c r="AD37" s="14"/>
     </row>
     <row r="38" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="150"/>
+      <c r="A38" s="120"/>
       <c r="B38" s="55"/>
-      <c r="C38" s="147" t="s">
+      <c r="C38" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="147"/>
-      <c r="E38" s="147"/>
-      <c r="F38" s="147"/>
-      <c r="G38" s="147"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="151"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="151"/>
-      <c r="L38" s="151"/>
-      <c r="M38" s="151"/>
-      <c r="N38" s="151"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="140"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="125"/>
+      <c r="J38" s="125"/>
+      <c r="K38" s="125"/>
+      <c r="L38" s="125"/>
+      <c r="M38" s="125"/>
+      <c r="N38" s="125"/>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
-      <c r="R38" s="143"/>
-      <c r="S38" s="143"/>
-      <c r="T38" s="143"/>
-      <c r="U38" s="143"/>
-      <c r="V38" s="143"/>
-      <c r="W38" s="143"/>
-      <c r="X38" s="143"/>
-      <c r="Y38" s="143"/>
-      <c r="Z38" s="143"/>
-      <c r="AA38" s="143"/>
-      <c r="AB38" s="143"/>
+      <c r="R38" s="136"/>
+      <c r="S38" s="136"/>
+      <c r="T38" s="136"/>
+      <c r="U38" s="136"/>
+      <c r="V38" s="136"/>
+      <c r="W38" s="136"/>
+      <c r="X38" s="136"/>
+      <c r="Y38" s="136"/>
+      <c r="Z38" s="136"/>
+      <c r="AA38" s="136"/>
+      <c r="AB38" s="136"/>
       <c r="AC38" s="47"/>
       <c r="AD38" s="14"/>
     </row>
     <row r="39" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="150"/>
+      <c r="A39" s="120"/>
       <c r="B39" s="55"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="148"/>
-      <c r="F39" s="148"/>
-      <c r="G39" s="148"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="152" t="s">
+      <c r="C39" s="141"/>
+      <c r="D39" s="141"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="141"/>
+      <c r="G39" s="141"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="J39" s="152"/>
+      <c r="J39" s="107"/>
       <c r="K39" s="45"/>
-      <c r="L39" s="152" t="s">
+      <c r="L39" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="M39" s="152"/>
-      <c r="N39" s="152"/>
+      <c r="M39" s="107"/>
+      <c r="N39" s="107"/>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
-      <c r="R39" s="152" t="s">
+      <c r="R39" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="S39" s="152"/>
-      <c r="T39" s="152"/>
+      <c r="S39" s="107"/>
+      <c r="T39" s="107"/>
       <c r="U39" s="46"/>
       <c r="V39" s="46"/>
       <c r="W39" s="46"/>
-      <c r="X39" s="152" t="s">
+      <c r="X39" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="Y39" s="152"/>
-      <c r="Z39" s="152"/>
-      <c r="AA39" s="152"/>
+      <c r="Y39" s="107"/>
+      <c r="Z39" s="107"/>
+      <c r="AA39" s="107"/>
       <c r="AB39" s="46"/>
       <c r="AC39" s="47"/>
       <c r="AD39" s="14"/>
     </row>
     <row r="40" spans="1:30" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="150"/>
+      <c r="A40" s="120"/>
       <c r="B40" s="55"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="85"/>
-      <c r="G40" s="85"/>
-      <c r="H40" s="85"/>
-      <c r="I40" s="142" t="s">
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="J40" s="142"/>
+      <c r="J40" s="124"/>
       <c r="K40" s="12"/>
-      <c r="L40" s="142" t="s">
+      <c r="L40" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="M40" s="142"/>
-      <c r="N40" s="142"/>
+      <c r="M40" s="124"/>
+      <c r="N40" s="124"/>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
-      <c r="R40" s="142" t="s">
+      <c r="R40" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="S40" s="142"/>
+      <c r="S40" s="124"/>
       <c r="T40" s="48"/>
       <c r="U40" s="48"/>
       <c r="V40" s="48"/>
@@ -2905,311 +2924,311 @@
       <c r="AD40" s="6"/>
     </row>
     <row r="41" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="150"/>
+      <c r="A41" s="120"/>
       <c r="B41" s="55"/>
-      <c r="C41" s="153" t="s">
+      <c r="C41" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="153"/>
-      <c r="E41" s="153"/>
-      <c r="F41" s="153"/>
-      <c r="G41" s="153"/>
-      <c r="H41" s="153"/>
-      <c r="I41" s="90" t="s">
+      <c r="D41" s="99"/>
+      <c r="E41" s="99"/>
+      <c r="F41" s="99"/>
+      <c r="G41" s="99"/>
+      <c r="H41" s="99"/>
+      <c r="I41" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="J41" s="75"/>
+      <c r="J41" s="74"/>
       <c r="K41" s="12"/>
-      <c r="L41" s="76" t="s">
+      <c r="L41" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="M41" s="74"/>
-      <c r="N41" s="75"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="74"/>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
-      <c r="R41" s="76" t="s">
+      <c r="R41" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="S41" s="74"/>
-      <c r="T41" s="75"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="74"/>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
-      <c r="X41" s="76" t="s">
+      <c r="X41" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="Y41" s="74"/>
-      <c r="Z41" s="77"/>
-      <c r="AA41" s="78"/>
+      <c r="Y41" s="73"/>
+      <c r="Z41" s="76"/>
+      <c r="AA41" s="77"/>
       <c r="AB41" s="26"/>
       <c r="AC41" s="51"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A42" s="150"/>
+      <c r="A42" s="120"/>
       <c r="B42" s="55"/>
-      <c r="C42" s="153"/>
-      <c r="D42" s="153"/>
-      <c r="E42" s="153"/>
-      <c r="F42" s="153"/>
-      <c r="G42" s="153"/>
-      <c r="H42" s="153"/>
-      <c r="I42" s="124"/>
-      <c r="J42" s="126"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="99"/>
+      <c r="I42" s="104"/>
+      <c r="J42" s="106"/>
       <c r="K42" s="12"/>
-      <c r="L42" s="124"/>
-      <c r="M42" s="125"/>
-      <c r="N42" s="126"/>
+      <c r="L42" s="104"/>
+      <c r="M42" s="105"/>
+      <c r="N42" s="106"/>
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
-      <c r="R42" s="115">
+      <c r="R42" s="121">
         <v>0</v>
       </c>
-      <c r="S42" s="116"/>
-      <c r="T42" s="117"/>
+      <c r="S42" s="122"/>
+      <c r="T42" s="123"/>
       <c r="U42" s="22"/>
       <c r="V42" s="12"/>
       <c r="W42" s="12"/>
-      <c r="X42" s="115">
+      <c r="X42" s="121">
         <v>0</v>
       </c>
-      <c r="Y42" s="116"/>
-      <c r="Z42" s="116"/>
-      <c r="AA42" s="117"/>
+      <c r="Y42" s="122"/>
+      <c r="Z42" s="122"/>
+      <c r="AA42" s="123"/>
       <c r="AB42" s="12"/>
       <c r="AC42" s="31"/>
     </row>
     <row r="43" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="150"/>
+      <c r="A43" s="120"/>
       <c r="B43" s="55"/>
-      <c r="C43" s="153" t="s">
+      <c r="C43" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="153"/>
-      <c r="E43" s="153"/>
-      <c r="F43" s="153"/>
-      <c r="G43" s="153"/>
-      <c r="H43" s="153"/>
-      <c r="I43" s="76" t="s">
+      <c r="D43" s="99"/>
+      <c r="E43" s="99"/>
+      <c r="F43" s="99"/>
+      <c r="G43" s="99"/>
+      <c r="H43" s="99"/>
+      <c r="I43" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="75"/>
+      <c r="J43" s="74"/>
       <c r="K43" s="12"/>
-      <c r="L43" s="76" t="s">
+      <c r="L43" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="M43" s="79"/>
-      <c r="N43" s="75"/>
+      <c r="M43" s="78"/>
+      <c r="N43" s="74"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
-      <c r="R43" s="76" t="s">
+      <c r="R43" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="S43" s="74"/>
-      <c r="T43" s="75"/>
+      <c r="S43" s="73"/>
+      <c r="T43" s="74"/>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
-      <c r="X43" s="76" t="s">
+      <c r="X43" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="Y43" s="74"/>
-      <c r="Z43" s="77"/>
-      <c r="AA43" s="78"/>
+      <c r="Y43" s="73"/>
+      <c r="Z43" s="76"/>
+      <c r="AA43" s="77"/>
       <c r="AB43" s="26"/>
       <c r="AC43" s="51"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A44" s="150"/>
+      <c r="A44" s="120"/>
       <c r="B44" s="55"/>
-      <c r="C44" s="153"/>
-      <c r="D44" s="153"/>
-      <c r="E44" s="153"/>
-      <c r="F44" s="153"/>
-      <c r="G44" s="153"/>
-      <c r="H44" s="153"/>
-      <c r="I44" s="124"/>
-      <c r="J44" s="126"/>
+      <c r="C44" s="99"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="99"/>
+      <c r="F44" s="99"/>
+      <c r="G44" s="99"/>
+      <c r="H44" s="99"/>
+      <c r="I44" s="104"/>
+      <c r="J44" s="106"/>
       <c r="K44" s="12"/>
-      <c r="L44" s="124"/>
-      <c r="M44" s="125"/>
-      <c r="N44" s="126"/>
+      <c r="L44" s="104"/>
+      <c r="M44" s="105"/>
+      <c r="N44" s="106"/>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
-      <c r="R44" s="115">
+      <c r="R44" s="121">
         <v>0</v>
       </c>
-      <c r="S44" s="116"/>
-      <c r="T44" s="117"/>
+      <c r="S44" s="122"/>
+      <c r="T44" s="123"/>
       <c r="U44" s="13"/>
       <c r="V44" s="12"/>
       <c r="W44" s="12"/>
-      <c r="X44" s="115">
+      <c r="X44" s="121">
         <v>0</v>
       </c>
-      <c r="Y44" s="116"/>
-      <c r="Z44" s="116"/>
-      <c r="AA44" s="117"/>
+      <c r="Y44" s="122"/>
+      <c r="Z44" s="122"/>
+      <c r="AA44" s="123"/>
       <c r="AB44" s="12"/>
       <c r="AC44" s="31"/>
     </row>
     <row r="45" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="150"/>
+      <c r="A45" s="120"/>
       <c r="B45" s="55"/>
-      <c r="C45" s="153" t="s">
+      <c r="C45" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="153"/>
-      <c r="E45" s="153"/>
-      <c r="F45" s="153"/>
-      <c r="G45" s="153"/>
-      <c r="H45" s="153"/>
-      <c r="I45" s="76" t="s">
+      <c r="D45" s="99"/>
+      <c r="E45" s="99"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="99"/>
+      <c r="H45" s="99"/>
+      <c r="I45" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="J45" s="80"/>
+      <c r="J45" s="79"/>
       <c r="K45" s="12"/>
-      <c r="L45" s="76" t="s">
+      <c r="L45" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="M45" s="74"/>
-      <c r="N45" s="75"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="74"/>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="12"/>
-      <c r="R45" s="76" t="s">
+      <c r="R45" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="S45" s="74"/>
-      <c r="T45" s="75"/>
+      <c r="S45" s="73"/>
+      <c r="T45" s="74"/>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
-      <c r="X45" s="76" t="s">
+      <c r="X45" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="Y45" s="74"/>
-      <c r="Z45" s="77"/>
-      <c r="AA45" s="78"/>
+      <c r="Y45" s="73"/>
+      <c r="Z45" s="76"/>
+      <c r="AA45" s="77"/>
       <c r="AB45" s="26"/>
       <c r="AC45" s="51"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A46" s="150"/>
+      <c r="A46" s="120"/>
       <c r="B46" s="55"/>
-      <c r="C46" s="153"/>
-      <c r="D46" s="153"/>
-      <c r="E46" s="153"/>
-      <c r="F46" s="153"/>
-      <c r="G46" s="153"/>
-      <c r="H46" s="153"/>
-      <c r="I46" s="124"/>
-      <c r="J46" s="126"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="99"/>
+      <c r="F46" s="99"/>
+      <c r="G46" s="99"/>
+      <c r="H46" s="99"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="106"/>
       <c r="K46" s="12"/>
-      <c r="L46" s="124"/>
-      <c r="M46" s="125"/>
-      <c r="N46" s="126"/>
+      <c r="L46" s="104"/>
+      <c r="M46" s="105"/>
+      <c r="N46" s="106"/>
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="12"/>
-      <c r="R46" s="115">
+      <c r="R46" s="121">
         <v>0</v>
       </c>
-      <c r="S46" s="116"/>
-      <c r="T46" s="117"/>
+      <c r="S46" s="122"/>
+      <c r="T46" s="123"/>
       <c r="U46" s="13"/>
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
-      <c r="X46" s="115">
+      <c r="X46" s="121">
         <v>0</v>
       </c>
-      <c r="Y46" s="116"/>
-      <c r="Z46" s="116"/>
-      <c r="AA46" s="117"/>
+      <c r="Y46" s="122"/>
+      <c r="Z46" s="122"/>
+      <c r="AA46" s="123"/>
       <c r="AB46" s="12"/>
       <c r="AC46" s="31"/>
     </row>
     <row r="47" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="150"/>
+      <c r="A47" s="120"/>
       <c r="B47" s="55"/>
-      <c r="C47" s="153" t="s">
+      <c r="C47" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="153"/>
-      <c r="E47" s="153"/>
-      <c r="F47" s="153"/>
-      <c r="G47" s="153"/>
-      <c r="H47" s="153"/>
-      <c r="I47" s="76" t="s">
+      <c r="D47" s="99"/>
+      <c r="E47" s="99"/>
+      <c r="F47" s="99"/>
+      <c r="G47" s="99"/>
+      <c r="H47" s="99"/>
+      <c r="I47" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="J47" s="80"/>
+      <c r="J47" s="79"/>
       <c r="K47" s="12"/>
-      <c r="L47" s="76" t="s">
+      <c r="L47" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="M47" s="74"/>
-      <c r="N47" s="75"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="74"/>
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="12"/>
-      <c r="R47" s="76" t="s">
+      <c r="R47" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="S47" s="87"/>
-      <c r="T47" s="75"/>
+      <c r="S47" s="85"/>
+      <c r="T47" s="74"/>
       <c r="U47" s="12"/>
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
-      <c r="X47" s="76" t="s">
+      <c r="X47" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="Y47" s="74"/>
-      <c r="Z47" s="77"/>
-      <c r="AA47" s="78"/>
+      <c r="Y47" s="73"/>
+      <c r="Z47" s="76"/>
+      <c r="AA47" s="77"/>
       <c r="AB47" s="26"/>
       <c r="AC47" s="51"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A48" s="150"/>
+      <c r="A48" s="120"/>
       <c r="B48" s="55"/>
-      <c r="C48" s="153"/>
-      <c r="D48" s="153"/>
-      <c r="E48" s="153"/>
-      <c r="F48" s="153"/>
-      <c r="G48" s="153"/>
-      <c r="H48" s="153"/>
-      <c r="I48" s="124"/>
-      <c r="J48" s="126"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="99"/>
+      <c r="G48" s="99"/>
+      <c r="H48" s="99"/>
+      <c r="I48" s="104"/>
+      <c r="J48" s="106"/>
       <c r="K48" s="12"/>
-      <c r="L48" s="124"/>
-      <c r="M48" s="125"/>
-      <c r="N48" s="126"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="105"/>
+      <c r="N48" s="106"/>
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="12"/>
-      <c r="R48" s="115">
+      <c r="R48" s="121">
         <v>0</v>
       </c>
-      <c r="S48" s="116"/>
-      <c r="T48" s="117"/>
+      <c r="S48" s="122"/>
+      <c r="T48" s="123"/>
       <c r="U48" s="13"/>
       <c r="V48" s="12"/>
       <c r="W48" s="12"/>
-      <c r="X48" s="115">
+      <c r="X48" s="121">
         <v>0</v>
       </c>
-      <c r="Y48" s="116"/>
-      <c r="Z48" s="116"/>
-      <c r="AA48" s="117"/>
+      <c r="Y48" s="122"/>
+      <c r="Z48" s="122"/>
+      <c r="AA48" s="123"/>
       <c r="AB48" s="12"/>
       <c r="AC48" s="31"/>
     </row>
     <row r="49" spans="1:29" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="150"/>
+      <c r="A49" s="120"/>
       <c r="B49" s="55"/>
       <c r="C49" s="52"/>
       <c r="D49" s="52"/>
@@ -3240,7 +3259,7 @@
       <c r="AC49" s="31"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A50" s="150"/>
+      <c r="A50" s="120"/>
       <c r="B50" s="55"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -3265,7 +3284,7 @@
       <c r="U50" s="10"/>
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
-      <c r="X50" s="91" t="s">
+      <c r="X50" s="89" t="s">
         <v>70</v>
       </c>
       <c r="Y50" s="9"/>
@@ -3275,7 +3294,7 @@
       <c r="AC50" s="31"/>
     </row>
     <row r="51" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="150"/>
+      <c r="A51" s="120"/>
       <c r="B51" s="55"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -3292,25 +3311,25 @@
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="53"/>
-      <c r="R51" s="95">
+      <c r="R51" s="93">
         <v>0</v>
       </c>
-      <c r="S51" s="96"/>
-      <c r="T51" s="96"/>
-      <c r="U51" s="97"/>
+      <c r="S51" s="94"/>
+      <c r="T51" s="94"/>
+      <c r="U51" s="95"/>
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
-      <c r="X51" s="95">
+      <c r="X51" s="93">
         <v>0</v>
       </c>
-      <c r="Y51" s="96"/>
-      <c r="Z51" s="96"/>
-      <c r="AA51" s="96"/>
-      <c r="AB51" s="97"/>
+      <c r="Y51" s="94"/>
+      <c r="Z51" s="94"/>
+      <c r="AA51" s="94"/>
+      <c r="AB51" s="95"/>
       <c r="AC51" s="31"/>
     </row>
     <row r="52" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="150"/>
+      <c r="A52" s="120"/>
       <c r="B52" s="55"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -3327,21 +3346,21 @@
       <c r="O52" s="12"/>
       <c r="P52" s="53"/>
       <c r="Q52" s="53"/>
-      <c r="R52" s="98"/>
-      <c r="S52" s="99"/>
-      <c r="T52" s="99"/>
-      <c r="U52" s="100"/>
+      <c r="R52" s="96"/>
+      <c r="S52" s="97"/>
+      <c r="T52" s="97"/>
+      <c r="U52" s="98"/>
       <c r="V52" s="12"/>
       <c r="W52" s="12"/>
-      <c r="X52" s="98"/>
-      <c r="Y52" s="99"/>
-      <c r="Z52" s="99"/>
-      <c r="AA52" s="99"/>
-      <c r="AB52" s="100"/>
+      <c r="X52" s="96"/>
+      <c r="Y52" s="97"/>
+      <c r="Z52" s="97"/>
+      <c r="AA52" s="97"/>
+      <c r="AB52" s="98"/>
       <c r="AC52" s="31"/>
     </row>
     <row r="53" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="150"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="55"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -3372,7 +3391,7 @@
       <c r="AC53" s="31"/>
     </row>
     <row r="54" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="150"/>
+      <c r="A54" s="120"/>
       <c r="B54" s="55"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -3395,7 +3414,7 @@
       <c r="U54" s="12"/>
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
-      <c r="X54" s="91" t="s">
+      <c r="X54" s="89" t="s">
         <v>71</v>
       </c>
       <c r="Y54" s="9"/>
@@ -3405,7 +3424,7 @@
       <c r="AC54" s="31"/>
     </row>
     <row r="55" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="150"/>
+      <c r="A55" s="120"/>
       <c r="B55" s="55"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
@@ -3428,15 +3447,15 @@
       <c r="U55" s="12"/>
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
-      <c r="X55" s="93"/>
-      <c r="Y55" s="92"/>
-      <c r="Z55" s="92"/>
-      <c r="AA55" s="92"/>
-      <c r="AB55" s="94"/>
+      <c r="X55" s="91"/>
+      <c r="Y55" s="90"/>
+      <c r="Z55" s="90"/>
+      <c r="AA55" s="90"/>
+      <c r="AB55" s="92"/>
       <c r="AC55" s="31"/>
     </row>
     <row r="56" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="150"/>
+      <c r="A56" s="120"/>
       <c r="B56" s="55"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -3459,25 +3478,25 @@
       <c r="U56" s="12"/>
       <c r="V56" s="12"/>
       <c r="W56" s="12"/>
-      <c r="X56" s="95">
+      <c r="X56" s="93">
         <v>0</v>
       </c>
-      <c r="Y56" s="96"/>
-      <c r="Z56" s="96"/>
-      <c r="AA56" s="96"/>
-      <c r="AB56" s="97"/>
+      <c r="Y56" s="94"/>
+      <c r="Z56" s="94"/>
+      <c r="AA56" s="94"/>
+      <c r="AB56" s="95"/>
       <c r="AC56" s="31"/>
     </row>
     <row r="57" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="150"/>
-      <c r="X57" s="98"/>
-      <c r="Y57" s="99"/>
-      <c r="Z57" s="99"/>
-      <c r="AA57" s="99"/>
-      <c r="AB57" s="100"/>
+      <c r="A57" s="120"/>
+      <c r="X57" s="96"/>
+      <c r="Y57" s="97"/>
+      <c r="Z57" s="97"/>
+      <c r="AA57" s="97"/>
+      <c r="AB57" s="98"/>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A58" s="150"/>
+      <c r="A58" s="120"/>
       <c r="B58" s="55"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -3485,36 +3504,36 @@
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="101" t="s">
+      <c r="I58" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="J58" s="101"/>
-      <c r="K58" s="101"/>
-      <c r="L58" s="101"/>
-      <c r="M58" s="101"/>
-      <c r="N58" s="101"/>
-      <c r="O58" s="101"/>
-      <c r="P58" s="101"/>
+      <c r="J58" s="148"/>
+      <c r="K58" s="148"/>
+      <c r="L58" s="148"/>
+      <c r="M58" s="148"/>
+      <c r="N58" s="148"/>
+      <c r="O58" s="148"/>
+      <c r="P58" s="148"/>
       <c r="Q58" s="12"/>
-      <c r="R58" s="76" t="s">
+      <c r="R58" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="S58" s="74"/>
-      <c r="T58" s="74"/>
-      <c r="U58" s="75"/>
+      <c r="S58" s="73"/>
+      <c r="T58" s="73"/>
+      <c r="U58" s="74"/>
       <c r="V58" s="12"/>
       <c r="W58" s="12"/>
-      <c r="X58" s="76" t="s">
+      <c r="X58" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="Y58" s="74"/>
-      <c r="Z58" s="74"/>
-      <c r="AA58" s="74"/>
-      <c r="AB58" s="75"/>
+      <c r="Y58" s="73"/>
+      <c r="Z58" s="73"/>
+      <c r="AA58" s="73"/>
+      <c r="AB58" s="74"/>
       <c r="AC58" s="31"/>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A59" s="150"/>
+      <c r="A59" s="120"/>
       <c r="B59" s="55"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
@@ -3522,34 +3541,34 @@
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="101"/>
-      <c r="J59" s="101"/>
-      <c r="K59" s="101"/>
-      <c r="L59" s="101"/>
-      <c r="M59" s="101"/>
-      <c r="N59" s="101"/>
-      <c r="O59" s="101"/>
-      <c r="P59" s="101"/>
+      <c r="I59" s="148"/>
+      <c r="J59" s="148"/>
+      <c r="K59" s="148"/>
+      <c r="L59" s="148"/>
+      <c r="M59" s="148"/>
+      <c r="N59" s="148"/>
+      <c r="O59" s="148"/>
+      <c r="P59" s="148"/>
       <c r="Q59" s="54"/>
-      <c r="R59" s="115">
+      <c r="R59" s="121">
         <v>0</v>
       </c>
-      <c r="S59" s="116"/>
-      <c r="T59" s="116"/>
-      <c r="U59" s="117"/>
+      <c r="S59" s="122"/>
+      <c r="T59" s="122"/>
+      <c r="U59" s="123"/>
       <c r="V59" s="12"/>
       <c r="W59" s="12"/>
-      <c r="X59" s="115">
+      <c r="X59" s="121">
         <v>0</v>
       </c>
-      <c r="Y59" s="116"/>
-      <c r="Z59" s="116"/>
-      <c r="AA59" s="116"/>
-      <c r="AB59" s="117"/>
+      <c r="Y59" s="122"/>
+      <c r="Z59" s="122"/>
+      <c r="AA59" s="122"/>
+      <c r="AB59" s="123"/>
       <c r="AC59" s="31"/>
     </row>
     <row r="60" spans="1:29" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="150"/>
+      <c r="A60" s="120"/>
       <c r="B60" s="55"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -3580,7 +3599,7 @@
       <c r="AC60" s="31"/>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A61" s="150"/>
+      <c r="A61" s="120"/>
       <c r="B61" s="55"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -3615,7 +3634,7 @@
       <c r="AC61" s="31"/>
     </row>
     <row r="62" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="150"/>
+      <c r="A62" s="120"/>
       <c r="B62" s="55"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
@@ -3632,27 +3651,25 @@
       <c r="O62" s="12"/>
       <c r="P62" s="53"/>
       <c r="Q62" s="53"/>
-      <c r="R62" s="130">
-        <f>IF(R51&gt;R59,R51,R59)</f>
+      <c r="R62" s="142">
         <v>0</v>
       </c>
-      <c r="S62" s="96"/>
-      <c r="T62" s="131"/>
+      <c r="S62" s="94"/>
+      <c r="T62" s="143"/>
       <c r="U62" s="12"/>
       <c r="V62" s="12"/>
       <c r="W62" s="12"/>
-      <c r="X62" s="130">
-        <f>IF(X51&gt;X59,X51,X59)</f>
+      <c r="X62" s="142">
         <v>0</v>
       </c>
-      <c r="Y62" s="96"/>
-      <c r="Z62" s="96"/>
-      <c r="AA62" s="131"/>
+      <c r="Y62" s="94"/>
+      <c r="Z62" s="94"/>
+      <c r="AA62" s="143"/>
       <c r="AB62" s="12"/>
       <c r="AC62" s="31"/>
     </row>
     <row r="63" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="150"/>
+      <c r="A63" s="120"/>
       <c r="B63" s="55"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
@@ -3669,22 +3686,22 @@
       <c r="O63" s="12"/>
       <c r="P63" s="53"/>
       <c r="Q63" s="53"/>
-      <c r="R63" s="132"/>
-      <c r="S63" s="133"/>
-      <c r="T63" s="134"/>
+      <c r="R63" s="144"/>
+      <c r="S63" s="145"/>
+      <c r="T63" s="146"/>
       <c r="U63" s="12"/>
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
-      <c r="X63" s="132"/>
-      <c r="Y63" s="133"/>
-      <c r="Z63" s="133"/>
-      <c r="AA63" s="134"/>
+      <c r="X63" s="144"/>
+      <c r="Y63" s="145"/>
+      <c r="Z63" s="145"/>
+      <c r="AA63" s="146"/>
       <c r="AB63" s="12"/>
       <c r="AC63" s="31"/>
     </row>
     <row r="64" spans="1:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="150"/>
-      <c r="B64" s="89"/>
+      <c r="A64" s="120"/>
+      <c r="B64" s="87"/>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
       <c r="E64" s="35"/>
@@ -3745,7 +3762,7 @@
       <c r="AC65" s="12"/>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A66" s="149" t="s">
+      <c r="A66" s="111" t="s">
         <v>42</v>
       </c>
       <c r="B66" s="40"/>
@@ -3780,7 +3797,7 @@
       <c r="AC66" s="10"/>
     </row>
     <row r="67" spans="1:30" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="149"/>
+      <c r="A67" s="111"/>
       <c r="B67" s="30"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -3811,35 +3828,35 @@
       <c r="AC67" s="31"/>
     </row>
     <row r="68" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="149"/>
+      <c r="A68" s="111"/>
       <c r="B68" s="30"/>
-      <c r="C68" s="135" t="s">
+      <c r="C68" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="135"/>
-      <c r="E68" s="135"/>
-      <c r="F68" s="135"/>
-      <c r="G68" s="135"/>
-      <c r="H68" s="135"/>
-      <c r="I68" s="135"/>
-      <c r="J68" s="135"/>
-      <c r="K68" s="135"/>
-      <c r="L68" s="135"/>
+      <c r="D68" s="100"/>
+      <c r="E68" s="100"/>
+      <c r="F68" s="100"/>
+      <c r="G68" s="100"/>
+      <c r="H68" s="100"/>
+      <c r="I68" s="100"/>
+      <c r="J68" s="100"/>
+      <c r="K68" s="100"/>
+      <c r="L68" s="100"/>
       <c r="M68" s="12"/>
-      <c r="N68" s="114" t="s">
+      <c r="N68" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="O68" s="114"/>
-      <c r="P68" s="114"/>
-      <c r="Q68" s="114"/>
-      <c r="R68" s="114"/>
-      <c r="S68" s="114"/>
-      <c r="T68" s="114"/>
-      <c r="U68" s="114"/>
-      <c r="V68" s="114"/>
-      <c r="W68" s="114"/>
-      <c r="X68" s="114"/>
-      <c r="Y68" s="114"/>
+      <c r="O68" s="147"/>
+      <c r="P68" s="147"/>
+      <c r="Q68" s="147"/>
+      <c r="R68" s="147"/>
+      <c r="S68" s="147"/>
+      <c r="T68" s="147"/>
+      <c r="U68" s="147"/>
+      <c r="V68" s="147"/>
+      <c r="W68" s="147"/>
+      <c r="X68" s="147"/>
+      <c r="Y68" s="147"/>
       <c r="Z68" s="8" t="s">
         <v>47</v>
       </c>
@@ -3848,41 +3865,41 @@
       <c r="AC68" s="51"/>
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A69" s="149"/>
+      <c r="A69" s="111"/>
       <c r="B69" s="30"/>
-      <c r="C69" s="135"/>
-      <c r="D69" s="135"/>
-      <c r="E69" s="135"/>
-      <c r="F69" s="135"/>
-      <c r="G69" s="135"/>
-      <c r="H69" s="135"/>
-      <c r="I69" s="135"/>
-      <c r="J69" s="135"/>
-      <c r="K69" s="135"/>
-      <c r="L69" s="135"/>
+      <c r="C69" s="100"/>
+      <c r="D69" s="100"/>
+      <c r="E69" s="100"/>
+      <c r="F69" s="100"/>
+      <c r="G69" s="100"/>
+      <c r="H69" s="100"/>
+      <c r="I69" s="100"/>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+      <c r="L69" s="100"/>
       <c r="M69" s="12"/>
-      <c r="N69" s="114"/>
-      <c r="O69" s="114"/>
-      <c r="P69" s="114"/>
-      <c r="Q69" s="114"/>
-      <c r="R69" s="114"/>
-      <c r="S69" s="114"/>
-      <c r="T69" s="114"/>
-      <c r="U69" s="114"/>
-      <c r="V69" s="114"/>
-      <c r="W69" s="114"/>
-      <c r="X69" s="114"/>
-      <c r="Y69" s="114"/>
-      <c r="Z69" s="111" t="str">
+      <c r="N69" s="147"/>
+      <c r="O69" s="147"/>
+      <c r="P69" s="147"/>
+      <c r="Q69" s="147"/>
+      <c r="R69" s="147"/>
+      <c r="S69" s="147"/>
+      <c r="T69" s="147"/>
+      <c r="U69" s="147"/>
+      <c r="V69" s="147"/>
+      <c r="W69" s="147"/>
+      <c r="X69" s="147"/>
+      <c r="Y69" s="147"/>
+      <c r="Z69" s="149" t="str">
         <f>IF(R62&gt;X62,R62-X62,"-")</f>
         <v>-</v>
       </c>
-      <c r="AA69" s="112"/>
-      <c r="AB69" s="113"/>
+      <c r="AA69" s="150"/>
+      <c r="AB69" s="151"/>
       <c r="AC69" s="31"/>
     </row>
     <row r="70" spans="1:30" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="149"/>
+      <c r="A70" s="111"/>
       <c r="B70" s="30"/>
       <c r="C70" s="56"/>
       <c r="D70" s="56"/>
@@ -3913,35 +3930,35 @@
       <c r="AC70" s="31"/>
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A71" s="149"/>
+      <c r="A71" s="111"/>
       <c r="B71" s="30"/>
-      <c r="C71" s="135" t="s">
+      <c r="C71" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="D71" s="135"/>
-      <c r="E71" s="135"/>
-      <c r="F71" s="135"/>
-      <c r="G71" s="135"/>
-      <c r="H71" s="135"/>
-      <c r="I71" s="135"/>
-      <c r="J71" s="135"/>
-      <c r="K71" s="135"/>
-      <c r="L71" s="135"/>
+      <c r="D71" s="100"/>
+      <c r="E71" s="100"/>
+      <c r="F71" s="100"/>
+      <c r="G71" s="100"/>
+      <c r="H71" s="100"/>
+      <c r="I71" s="100"/>
+      <c r="J71" s="100"/>
+      <c r="K71" s="100"/>
+      <c r="L71" s="100"/>
       <c r="M71" s="12"/>
-      <c r="N71" s="114" t="s">
+      <c r="N71" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="O71" s="114"/>
-      <c r="P71" s="114"/>
-      <c r="Q71" s="114"/>
-      <c r="R71" s="114"/>
-      <c r="S71" s="114"/>
-      <c r="T71" s="114"/>
-      <c r="U71" s="114"/>
-      <c r="V71" s="114"/>
-      <c r="W71" s="114"/>
-      <c r="X71" s="114"/>
-      <c r="Y71" s="114"/>
+      <c r="O71" s="147"/>
+      <c r="P71" s="147"/>
+      <c r="Q71" s="147"/>
+      <c r="R71" s="147"/>
+      <c r="S71" s="147"/>
+      <c r="T71" s="147"/>
+      <c r="U71" s="147"/>
+      <c r="V71" s="147"/>
+      <c r="W71" s="147"/>
+      <c r="X71" s="147"/>
+      <c r="Y71" s="147"/>
       <c r="Z71" s="8" t="s">
         <v>48</v>
       </c>
@@ -3950,41 +3967,41 @@
       <c r="AC71" s="51"/>
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A72" s="149"/>
+      <c r="A72" s="111"/>
       <c r="B72" s="30"/>
-      <c r="C72" s="135"/>
-      <c r="D72" s="135"/>
-      <c r="E72" s="135"/>
-      <c r="F72" s="135"/>
-      <c r="G72" s="135"/>
-      <c r="H72" s="135"/>
-      <c r="I72" s="135"/>
-      <c r="J72" s="135"/>
-      <c r="K72" s="135"/>
-      <c r="L72" s="135"/>
+      <c r="C72" s="100"/>
+      <c r="D72" s="100"/>
+      <c r="E72" s="100"/>
+      <c r="F72" s="100"/>
+      <c r="G72" s="100"/>
+      <c r="H72" s="100"/>
+      <c r="I72" s="100"/>
+      <c r="J72" s="100"/>
+      <c r="K72" s="100"/>
+      <c r="L72" s="100"/>
       <c r="M72" s="12"/>
-      <c r="N72" s="114"/>
-      <c r="O72" s="114"/>
-      <c r="P72" s="114"/>
-      <c r="Q72" s="114"/>
-      <c r="R72" s="114"/>
-      <c r="S72" s="114"/>
-      <c r="T72" s="114"/>
-      <c r="U72" s="114"/>
-      <c r="V72" s="114"/>
-      <c r="W72" s="114"/>
-      <c r="X72" s="114"/>
-      <c r="Y72" s="114"/>
-      <c r="Z72" s="111" t="str">
+      <c r="N72" s="147"/>
+      <c r="O72" s="147"/>
+      <c r="P72" s="147"/>
+      <c r="Q72" s="147"/>
+      <c r="R72" s="147"/>
+      <c r="S72" s="147"/>
+      <c r="T72" s="147"/>
+      <c r="U72" s="147"/>
+      <c r="V72" s="147"/>
+      <c r="W72" s="147"/>
+      <c r="X72" s="147"/>
+      <c r="Y72" s="147"/>
+      <c r="Z72" s="149" t="str">
         <f>IF(X62&gt;R62,X62-R62,"-")</f>
         <v>-</v>
       </c>
-      <c r="AA72" s="112"/>
-      <c r="AB72" s="113"/>
+      <c r="AA72" s="150"/>
+      <c r="AB72" s="151"/>
       <c r="AC72" s="31"/>
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A73" s="149"/>
+      <c r="A73" s="111"/>
       <c r="B73" s="34"/>
       <c r="C73" s="35"/>
       <c r="D73" s="35"/>
@@ -4022,142 +4039,142 @@
       <c r="E74" s="5"/>
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A75" s="149" t="s">
+      <c r="A75" s="111" t="s">
         <v>50</v>
       </c>
       <c r="B75" s="40"/>
-      <c r="C75" s="154" t="s">
+      <c r="C75" s="118" t="s">
         <v>73</v>
       </c>
-      <c r="D75" s="154"/>
-      <c r="E75" s="154"/>
-      <c r="F75" s="154"/>
-      <c r="G75" s="154"/>
-      <c r="H75" s="154"/>
-      <c r="I75" s="154"/>
-      <c r="J75" s="154"/>
-      <c r="K75" s="154"/>
-      <c r="L75" s="154"/>
-      <c r="M75" s="154"/>
-      <c r="N75" s="154"/>
-      <c r="O75" s="154"/>
-      <c r="P75" s="154"/>
-      <c r="Q75" s="154"/>
-      <c r="R75" s="154"/>
-      <c r="S75" s="154"/>
-      <c r="T75" s="154"/>
-      <c r="U75" s="154"/>
-      <c r="V75" s="154"/>
-      <c r="W75" s="154"/>
-      <c r="X75" s="154"/>
-      <c r="Y75" s="154"/>
-      <c r="Z75" s="154"/>
-      <c r="AA75" s="154"/>
-      <c r="AB75" s="154"/>
+      <c r="D75" s="118"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="118"/>
+      <c r="G75" s="118"/>
+      <c r="H75" s="118"/>
+      <c r="I75" s="118"/>
+      <c r="J75" s="118"/>
+      <c r="K75" s="118"/>
+      <c r="L75" s="118"/>
+      <c r="M75" s="118"/>
+      <c r="N75" s="118"/>
+      <c r="O75" s="118"/>
+      <c r="P75" s="118"/>
+      <c r="Q75" s="118"/>
+      <c r="R75" s="118"/>
+      <c r="S75" s="118"/>
+      <c r="T75" s="118"/>
+      <c r="U75" s="118"/>
+      <c r="V75" s="118"/>
+      <c r="W75" s="118"/>
+      <c r="X75" s="118"/>
+      <c r="Y75" s="118"/>
+      <c r="Z75" s="118"/>
+      <c r="AA75" s="118"/>
+      <c r="AB75" s="118"/>
       <c r="AC75" s="59"/>
       <c r="AD75" s="15"/>
     </row>
     <row r="76" spans="1:30" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="149"/>
+      <c r="A76" s="111"/>
       <c r="B76" s="30"/>
-      <c r="C76" s="155"/>
-      <c r="D76" s="155"/>
-      <c r="E76" s="155"/>
-      <c r="F76" s="155"/>
-      <c r="G76" s="155"/>
-      <c r="H76" s="155"/>
-      <c r="I76" s="155"/>
-      <c r="J76" s="155"/>
-      <c r="K76" s="155"/>
-      <c r="L76" s="155"/>
-      <c r="M76" s="155"/>
-      <c r="N76" s="155"/>
-      <c r="O76" s="155"/>
-      <c r="P76" s="155"/>
-      <c r="Q76" s="155"/>
-      <c r="R76" s="155"/>
-      <c r="S76" s="155"/>
-      <c r="T76" s="155"/>
-      <c r="U76" s="155"/>
-      <c r="V76" s="155"/>
-      <c r="W76" s="155"/>
-      <c r="X76" s="155"/>
-      <c r="Y76" s="155"/>
-      <c r="Z76" s="155"/>
-      <c r="AA76" s="155"/>
-      <c r="AB76" s="155"/>
+      <c r="C76" s="119"/>
+      <c r="D76" s="119"/>
+      <c r="E76" s="119"/>
+      <c r="F76" s="119"/>
+      <c r="G76" s="119"/>
+      <c r="H76" s="119"/>
+      <c r="I76" s="119"/>
+      <c r="J76" s="119"/>
+      <c r="K76" s="119"/>
+      <c r="L76" s="119"/>
+      <c r="M76" s="119"/>
+      <c r="N76" s="119"/>
+      <c r="O76" s="119"/>
+      <c r="P76" s="119"/>
+      <c r="Q76" s="119"/>
+      <c r="R76" s="119"/>
+      <c r="S76" s="119"/>
+      <c r="T76" s="119"/>
+      <c r="U76" s="119"/>
+      <c r="V76" s="119"/>
+      <c r="W76" s="119"/>
+      <c r="X76" s="119"/>
+      <c r="Y76" s="119"/>
+      <c r="Z76" s="119"/>
+      <c r="AA76" s="119"/>
+      <c r="AB76" s="119"/>
       <c r="AC76" s="60"/>
       <c r="AD76" s="15"/>
     </row>
     <row r="77" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="149"/>
+      <c r="A77" s="111"/>
       <c r="B77" s="30"/>
-      <c r="C77" s="76" t="s">
+      <c r="C77" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="74"/>
-      <c r="H77" s="74"/>
-      <c r="I77" s="74"/>
-      <c r="J77" s="74"/>
-      <c r="K77" s="74"/>
-      <c r="L77" s="74"/>
-      <c r="M77" s="74"/>
-      <c r="N77" s="74"/>
-      <c r="O77" s="74"/>
-      <c r="P77" s="75"/>
+      <c r="D77" s="73"/>
+      <c r="E77" s="73"/>
+      <c r="F77" s="73"/>
+      <c r="G77" s="73"/>
+      <c r="H77" s="73"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="73"/>
+      <c r="L77" s="73"/>
+      <c r="M77" s="73"/>
+      <c r="N77" s="73"/>
+      <c r="O77" s="73"/>
+      <c r="P77" s="74"/>
       <c r="Q77" s="12"/>
-      <c r="R77" s="82" t="s">
+      <c r="R77" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="S77" s="74"/>
-      <c r="T77" s="74"/>
-      <c r="U77" s="74"/>
-      <c r="V77" s="83"/>
-      <c r="W77" s="83"/>
-      <c r="X77" s="84"/>
-      <c r="Y77" s="84"/>
-      <c r="Z77" s="84"/>
-      <c r="AA77" s="84"/>
-      <c r="AB77" s="75"/>
+      <c r="S77" s="73"/>
+      <c r="T77" s="73"/>
+      <c r="U77" s="73"/>
+      <c r="V77" s="81"/>
+      <c r="W77" s="81"/>
+      <c r="X77" s="82"/>
+      <c r="Y77" s="82"/>
+      <c r="Z77" s="82"/>
+      <c r="AA77" s="82"/>
+      <c r="AB77" s="74"/>
       <c r="AC77" s="31"/>
     </row>
     <row r="78" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="149"/>
+      <c r="A78" s="111"/>
       <c r="B78" s="30"/>
-      <c r="C78" s="127"/>
-      <c r="D78" s="128"/>
-      <c r="E78" s="128"/>
-      <c r="F78" s="128"/>
-      <c r="G78" s="128"/>
-      <c r="H78" s="128"/>
-      <c r="I78" s="128"/>
-      <c r="J78" s="128"/>
-      <c r="K78" s="128"/>
-      <c r="L78" s="128"/>
-      <c r="M78" s="128"/>
-      <c r="N78" s="128"/>
-      <c r="O78" s="128"/>
-      <c r="P78" s="129"/>
+      <c r="C78" s="112"/>
+      <c r="D78" s="113"/>
+      <c r="E78" s="113"/>
+      <c r="F78" s="113"/>
+      <c r="G78" s="113"/>
+      <c r="H78" s="113"/>
+      <c r="I78" s="113"/>
+      <c r="J78" s="113"/>
+      <c r="K78" s="113"/>
+      <c r="L78" s="113"/>
+      <c r="M78" s="113"/>
+      <c r="N78" s="113"/>
+      <c r="O78" s="113"/>
+      <c r="P78" s="114"/>
       <c r="Q78" s="11"/>
-      <c r="R78" s="127"/>
-      <c r="S78" s="128"/>
-      <c r="T78" s="128"/>
-      <c r="U78" s="128"/>
-      <c r="V78" s="128"/>
-      <c r="W78" s="128"/>
-      <c r="X78" s="128"/>
-      <c r="Y78" s="128"/>
-      <c r="Z78" s="128"/>
-      <c r="AA78" s="128"/>
-      <c r="AB78" s="129"/>
+      <c r="R78" s="112"/>
+      <c r="S78" s="113"/>
+      <c r="T78" s="113"/>
+      <c r="U78" s="113"/>
+      <c r="V78" s="113"/>
+      <c r="W78" s="113"/>
+      <c r="X78" s="113"/>
+      <c r="Y78" s="113"/>
+      <c r="Z78" s="113"/>
+      <c r="AA78" s="113"/>
+      <c r="AB78" s="114"/>
       <c r="AC78" s="61"/>
       <c r="AD78" s="2"/>
     </row>
     <row r="79" spans="1:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="149"/>
+      <c r="A79" s="111"/>
       <c r="B79" s="30"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -4189,104 +4206,151 @@
       <c r="AD79" s="2"/>
     </row>
     <row r="80" spans="1:30" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="149"/>
+      <c r="A80" s="111"/>
       <c r="B80" s="30"/>
-      <c r="C80" s="76" t="s">
+      <c r="C80" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-      <c r="F80" s="74"/>
-      <c r="G80" s="74"/>
-      <c r="H80" s="74"/>
-      <c r="I80" s="74"/>
-      <c r="J80" s="74"/>
-      <c r="K80" s="74"/>
-      <c r="L80" s="74"/>
-      <c r="M80" s="74"/>
-      <c r="N80" s="74"/>
-      <c r="O80" s="74"/>
-      <c r="P80" s="75"/>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73"/>
+      <c r="F80" s="73"/>
+      <c r="G80" s="73"/>
+      <c r="H80" s="73"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="73"/>
+      <c r="M80" s="73"/>
+      <c r="N80" s="73"/>
+      <c r="O80" s="73"/>
+      <c r="P80" s="74"/>
       <c r="Q80" s="12"/>
-      <c r="R80" s="82" t="s">
+      <c r="R80" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="S80" s="74"/>
-      <c r="T80" s="74"/>
-      <c r="U80" s="74"/>
-      <c r="V80" s="83"/>
-      <c r="W80" s="83"/>
-      <c r="X80" s="84"/>
-      <c r="Y80" s="84"/>
-      <c r="Z80" s="84"/>
-      <c r="AA80" s="84"/>
-      <c r="AB80" s="75"/>
+      <c r="S80" s="73"/>
+      <c r="T80" s="73"/>
+      <c r="U80" s="73"/>
+      <c r="V80" s="81"/>
+      <c r="W80" s="81"/>
+      <c r="X80" s="82"/>
+      <c r="Y80" s="82"/>
+      <c r="Z80" s="82"/>
+      <c r="AA80" s="82"/>
+      <c r="AB80" s="74"/>
       <c r="AC80" s="31"/>
     </row>
     <row r="81" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="149"/>
+      <c r="A81" s="111"/>
       <c r="B81" s="30"/>
-      <c r="C81" s="156"/>
-      <c r="D81" s="157"/>
-      <c r="E81" s="157"/>
-      <c r="F81" s="157"/>
-      <c r="G81" s="157"/>
-      <c r="H81" s="157"/>
-      <c r="I81" s="157"/>
-      <c r="J81" s="157"/>
-      <c r="K81" s="157"/>
-      <c r="L81" s="157"/>
-      <c r="M81" s="157"/>
-      <c r="N81" s="157"/>
-      <c r="O81" s="157"/>
-      <c r="P81" s="158"/>
+      <c r="C81" s="115"/>
+      <c r="D81" s="116"/>
+      <c r="E81" s="116"/>
+      <c r="F81" s="116"/>
+      <c r="G81" s="116"/>
+      <c r="H81" s="116"/>
+      <c r="I81" s="116"/>
+      <c r="J81" s="116"/>
+      <c r="K81" s="116"/>
+      <c r="L81" s="116"/>
+      <c r="M81" s="116"/>
+      <c r="N81" s="116"/>
+      <c r="O81" s="116"/>
+      <c r="P81" s="117"/>
       <c r="Q81" s="13"/>
-      <c r="R81" s="108"/>
-      <c r="S81" s="109"/>
-      <c r="T81" s="109"/>
-      <c r="U81" s="109"/>
-      <c r="V81" s="109"/>
-      <c r="W81" s="109"/>
-      <c r="X81" s="109"/>
-      <c r="Y81" s="109"/>
-      <c r="Z81" s="109"/>
-      <c r="AA81" s="109"/>
-      <c r="AB81" s="110"/>
+      <c r="R81" s="101"/>
+      <c r="S81" s="102"/>
+      <c r="T81" s="102"/>
+      <c r="U81" s="102"/>
+      <c r="V81" s="102"/>
+      <c r="W81" s="102"/>
+      <c r="X81" s="102"/>
+      <c r="Y81" s="102"/>
+      <c r="Z81" s="102"/>
+      <c r="AA81" s="102"/>
+      <c r="AB81" s="103"/>
       <c r="AC81" s="61"/>
       <c r="AD81" s="2"/>
     </row>
-    <row r="82" spans="1:30" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="63"/>
-      <c r="C82" s="35"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="35"/>
-      <c r="J82" s="35"/>
-      <c r="K82" s="35"/>
-      <c r="L82" s="35"/>
-      <c r="M82" s="35"/>
-      <c r="N82" s="35"/>
-      <c r="O82" s="35"/>
-      <c r="P82" s="35"/>
-      <c r="Q82" s="35"/>
-      <c r="R82" s="35"/>
-      <c r="S82" s="35"/>
-      <c r="T82" s="35"/>
-      <c r="U82" s="35"/>
-      <c r="V82" s="35"/>
-      <c r="W82" s="35"/>
-      <c r="X82" s="35"/>
-      <c r="Y82" s="35"/>
-      <c r="Z82" s="81"/>
-      <c r="AA82" s="35"/>
-      <c r="AB82" s="35"/>
-      <c r="AC82" s="37"/>
+    <row r="82" spans="1:30" s="157" customFormat="1" ht="9" x14ac:dyDescent="0.15">
+      <c r="B82" s="158"/>
+      <c r="C82" s="159"/>
+      <c r="D82" s="159"/>
+      <c r="E82" s="159"/>
+      <c r="F82" s="159"/>
+      <c r="G82" s="159"/>
+      <c r="H82" s="159"/>
+      <c r="I82" s="159"/>
+      <c r="J82" s="159"/>
+      <c r="K82" s="159"/>
+      <c r="L82" s="159"/>
+      <c r="M82" s="159"/>
+      <c r="N82" s="159"/>
+      <c r="O82" s="159"/>
+      <c r="P82" s="159"/>
+      <c r="Q82" s="159"/>
+      <c r="R82" s="159"/>
+      <c r="S82" s="159"/>
+      <c r="T82" s="159"/>
+      <c r="U82" s="159"/>
+      <c r="V82" s="159"/>
+      <c r="W82" s="159"/>
+      <c r="X82" s="160">
+        <v>44384</v>
+      </c>
+      <c r="Y82" s="160"/>
+      <c r="Z82" s="160"/>
+      <c r="AA82" s="160"/>
+      <c r="AB82" s="160"/>
+      <c r="AC82" s="161"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="74">
+    <mergeCell ref="X82:AB82"/>
+    <mergeCell ref="Z72:AB72"/>
+    <mergeCell ref="N71:Y72"/>
+    <mergeCell ref="C71:L72"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="O6:AB6"/>
+    <mergeCell ref="C21:AB21"/>
+    <mergeCell ref="N2:AB4"/>
+    <mergeCell ref="A6:A28"/>
+    <mergeCell ref="P27:AB27"/>
+    <mergeCell ref="C38:G39"/>
+    <mergeCell ref="C24:AB24"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="X42:AA42"/>
+    <mergeCell ref="X46:AA46"/>
+    <mergeCell ref="X44:AA44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="R33:S33"/>
+    <mergeCell ref="T32:X33"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C12:AB12"/>
+    <mergeCell ref="C15:AB15"/>
+    <mergeCell ref="N18:V18"/>
+    <mergeCell ref="C18:L18"/>
+    <mergeCell ref="X18:AB18"/>
+    <mergeCell ref="C32:I33"/>
+    <mergeCell ref="M32:Q33"/>
+    <mergeCell ref="C27:N27"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="R39:T39"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I37:N38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R37:AB38"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="X39:AA39"/>
+    <mergeCell ref="N9:AB9"/>
     <mergeCell ref="A75:A81"/>
     <mergeCell ref="C78:P78"/>
     <mergeCell ref="C81:P81"/>
@@ -4294,77 +4358,33 @@
     <mergeCell ref="C41:H42"/>
     <mergeCell ref="C43:H44"/>
     <mergeCell ref="C75:AB76"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C12:AB12"/>
-    <mergeCell ref="C15:AB15"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="R46:T46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="R39:T39"/>
     <mergeCell ref="A66:A73"/>
     <mergeCell ref="A31:A64"/>
     <mergeCell ref="R48:T48"/>
     <mergeCell ref="X48:AA48"/>
     <mergeCell ref="R51:U52"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="L39:N39"/>
     <mergeCell ref="X51:AB52"/>
-    <mergeCell ref="I37:N38"/>
-    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C47:H48"/>
+    <mergeCell ref="C68:L69"/>
+    <mergeCell ref="R81:AB81"/>
     <mergeCell ref="C45:H46"/>
-    <mergeCell ref="C47:H48"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="X39:AA39"/>
-    <mergeCell ref="C68:L69"/>
-    <mergeCell ref="N9:AB9"/>
-    <mergeCell ref="N18:V18"/>
-    <mergeCell ref="C18:L18"/>
+    <mergeCell ref="X56:AB57"/>
+    <mergeCell ref="I48:J48"/>
     <mergeCell ref="I46:J46"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="C32:I33"/>
-    <mergeCell ref="M32:Q33"/>
-    <mergeCell ref="C27:N27"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R37:AB38"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="C38:G39"/>
-    <mergeCell ref="C24:AB24"/>
-    <mergeCell ref="P27:AB27"/>
-    <mergeCell ref="R81:AB81"/>
-    <mergeCell ref="Z69:AB69"/>
-    <mergeCell ref="Z72:AB72"/>
-    <mergeCell ref="N71:Y72"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="X42:AA42"/>
-    <mergeCell ref="X46:AA46"/>
-    <mergeCell ref="X44:AA44"/>
-    <mergeCell ref="L44:N44"/>
     <mergeCell ref="R78:AB78"/>
     <mergeCell ref="X59:AB59"/>
     <mergeCell ref="R62:T63"/>
     <mergeCell ref="X62:AA63"/>
     <mergeCell ref="R59:U59"/>
-    <mergeCell ref="C71:L72"/>
     <mergeCell ref="N68:Y69"/>
-    <mergeCell ref="X56:AB57"/>
     <mergeCell ref="I58:P59"/>
-    <mergeCell ref="A1:AC1"/>
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="O6:AB6"/>
-    <mergeCell ref="C21:AB21"/>
-    <mergeCell ref="N2:AB4"/>
-    <mergeCell ref="R33:S33"/>
-    <mergeCell ref="T32:X33"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="A6:A28"/>
+    <mergeCell ref="Z69:AB69"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup scale="94" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -4444,21 +4464,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E1A2E3E0B11A04FACDDAE56894BB66A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8495f4ae24506581391538332838489b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="89dd694e-5901-48c9-ab9f-04cf6a09355c" xmlns:ns4="f5499f45-605f-40a6-afd1-4be3d4a7469c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e994f2a63a8eefe28041002838a97de" ns3:_="" ns4:_="">
     <xsd:import namespace="89dd694e-5901-48c9-ab9f-04cf6a09355c"/>
@@ -4675,32 +4680,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8648CCD-298A-4C45-8E32-5224C118D136}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0A9BF63-3306-4D7C-B2B7-CB6DBD13122A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="89dd694e-5901-48c9-ab9f-04cf6a09355c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f5499f45-605f-40a6-afd1-4be3d4a7469c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D904A-8678-4187-93B5-FC6869F27369}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4717,4 +4712,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0A9BF63-3306-4D7C-B2B7-CB6DBD13122A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="89dd694e-5901-48c9-ab9f-04cf6a09355c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f5499f45-605f-40a6-afd1-4be3d4a7469c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8648CCD-298A-4C45-8E32-5224C118D136}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>